<commit_message>
more update. base models with target/no/ni/omic/algo/-> feature importances
</commit_message>
<xml_diff>
--- a/celltype_results_all.xlsx
+++ b/celltype_results_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebastien.delandtshe\PycharmProjects\DeepOncoAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD19640-A364-4D87-B64E-833C175E277B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539013A2-090D-4353-B0C4-1B6B36E19EAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="135" yWindow="285" windowWidth="27645" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="23010" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="celltype_results_all" sheetId="1" r:id="rId1"/>
@@ -1198,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AY17" sqref="AY17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,7 +1210,7 @@
     <col min="53" max="53" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="10" customFormat="1" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:47" s="10" customFormat="1" ht="124.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>

</xml_diff>